<commit_message>
Resolvido problemas de mapeamento
</commit_message>
<xml_diff>
--- a/BlazeAutomation/src/test/resources/massaDados.xlsx
+++ b/BlazeAutomation/src/test/resources/massaDados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JudrianideBrito\Desktop\PROJETO BRITO\assessment\BlazeAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4BD5E7-27AD-493B-921C-9E07DB1101A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F0B8A1-DA3A-4524-9F61-626EED5D38EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{93215AE1-DBF9-4410-B5CA-C1AC1697CFFC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="25">
   <si>
     <t>ID_0000</t>
   </si>
@@ -77,37 +77,40 @@
     <t>ID_0012</t>
   </si>
   <si>
+    <t>parametro 1</t>
+  </si>
+  <si>
+    <t>parametro 2</t>
+  </si>
+  <si>
+    <t>parametro 3</t>
+  </si>
+  <si>
+    <t>parametro 4</t>
+  </si>
+  <si>
+    <t>parametro 5</t>
+  </si>
+  <si>
+    <t>parametro 6</t>
+  </si>
+  <si>
+    <t>parametro 7</t>
+  </si>
+  <si>
+    <t>parametro 8</t>
+  </si>
+  <si>
+    <t>parametro 9</t>
+  </si>
+  <si>
+    <t>qualquer tipo</t>
+  </si>
+  <si>
     <t>clientevip@gmail.com</t>
   </si>
   <si>
-    <t>parametro 1</t>
-  </si>
-  <si>
-    <t>parametro 2</t>
-  </si>
-  <si>
-    <t>parametro 3</t>
-  </si>
-  <si>
-    <t>parametro 4</t>
-  </si>
-  <si>
-    <t>parametro 5</t>
-  </si>
-  <si>
-    <t>parametro 6</t>
-  </si>
-  <si>
-    <t>parametro 7</t>
-  </si>
-  <si>
-    <t>parametro 8</t>
-  </si>
-  <si>
-    <t>parametro 9</t>
-  </si>
-  <si>
-    <t>qualquer tipo</t>
+    <t>clienteviptwenty@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,13 +143,6 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -191,12 +187,11 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -516,22 +511,21 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -539,63 +533,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="C2" s="1">
         <v>241307241307</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -603,63 +597,63 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1">
+        <v>241307241307</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -667,31 +661,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -699,31 +693,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -731,31 +725,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -763,31 +757,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -795,31 +789,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -827,31 +821,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -859,31 +853,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -891,31 +885,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -923,39 +917,40 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{5600F807-6029-4E57-9993-1602AD6A27F9}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{0F22A87D-8BAE-4AA3-9F30-44EC8DE7229C}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Organizando codigo para entrega
</commit_message>
<xml_diff>
--- a/BlazeAutomation/src/test/resources/massaDados.xlsx
+++ b/BlazeAutomation/src/test/resources/massaDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JudrianideBrito\Desktop\PROJETO BRITO\assessment\BlazeAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCFFEC7-F367-41D5-90CD-416840062A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077E8D44-528D-4153-B694-EA1A41BDF57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{93215AE1-DBF9-4410-B5CA-C1AC1697CFFC}"/>
   </bookViews>
@@ -122,7 +122,7 @@
     <t>parametro 6</t>
   </si>
   <si>
-    <t>maria15fr5fddt</t>
+    <t>nomeNORMAL</t>
   </si>
 </sst>
 </file>
@@ -788,7 +788,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +998,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId5" name="Control 1">
+        <control shapeId="1029" r:id="rId5" name="Control 5">
           <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
@@ -1018,12 +1018,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId5" name="Control 1"/>
+        <control shapeId="1029" r:id="rId5" name="Control 5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId7" name="Control 2">
+        <control shapeId="1028" r:id="rId7" name="Control 4">
           <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
@@ -1043,7 +1043,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId7" name="Control 2"/>
+        <control shapeId="1028" r:id="rId7" name="Control 4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1073,7 +1073,7 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId9" name="Control 4">
+        <control shapeId="1026" r:id="rId9" name="Control 2">
           <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
@@ -1093,12 +1093,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId9" name="Control 4"/>
+        <control shapeId="1026" r:id="rId9" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId10" name="Control 5">
+        <control shapeId="1025" r:id="rId10" name="Control 1">
           <controlPr defaultSize="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
@@ -1118,7 +1118,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId10" name="Control 5"/>
+        <control shapeId="1025" r:id="rId10" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
implementado screenshot com sucesso!
</commit_message>
<xml_diff>
--- a/BlazeAutomation/src/test/resources/massaDados.xlsx
+++ b/BlazeAutomation/src/test/resources/massaDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JudrianideBrito\Desktop\PROJETO BRITO\assessment\BlazeAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077E8D44-528D-4153-B694-EA1A41BDF57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2F51A-F488-42F9-BA93-4F63DE2B91A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{93215AE1-DBF9-4410-B5CA-C1AC1697CFFC}"/>
   </bookViews>
@@ -122,7 +122,7 @@
     <t>parametro 6</t>
   </si>
   <si>
-    <t>nomeNORMAL</t>
+    <t>nomeNORMALd9</t>
   </si>
 </sst>
 </file>
@@ -788,7 +788,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>